<commit_message>
Correction to employment calculation in BEvIC
</commit_message>
<xml_diff>
--- a/InputData/io-model/BEbIC/BAU Employment by ISIC Code.xlsx
+++ b/InputData/io-model/BEbIC/BAU Employment by ISIC Code.xlsx
@@ -918,29 +918,20 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -969,14 +960,23 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1367,548 +1367,548 @@
       </c>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="35"/>
-      <c r="AF3" s="35"/>
-      <c r="AG3" s="35"/>
-      <c r="AH3" s="35"/>
-      <c r="AI3" s="35"/>
-      <c r="AJ3" s="35"/>
-      <c r="AK3" s="35"/>
-      <c r="AL3" s="35"/>
-      <c r="AM3" s="35"/>
-      <c r="AN3" s="35"/>
-      <c r="AO3" s="35"/>
-      <c r="AP3" s="35"/>
-      <c r="AQ3" s="35"/>
-      <c r="AR3" s="35"/>
-      <c r="AS3" s="35"/>
-      <c r="AT3" s="35"/>
-      <c r="AU3" s="35"/>
-      <c r="AV3" s="35"/>
-      <c r="AW3" s="35"/>
-      <c r="AX3" s="35"/>
-      <c r="AY3" s="35"/>
-      <c r="AZ3" s="35"/>
-      <c r="BA3" s="35"/>
-      <c r="BB3" s="35"/>
-      <c r="BC3" s="35"/>
-      <c r="BD3" s="35"/>
-      <c r="BE3" s="36"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="20"/>
+      <c r="AP3" s="20"/>
+      <c r="AQ3" s="20"/>
+      <c r="AR3" s="20"/>
+      <c r="AS3" s="20"/>
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="20"/>
+      <c r="AZ3" s="20"/>
+      <c r="BA3" s="20"/>
+      <c r="BB3" s="20"/>
+      <c r="BC3" s="20"/>
+      <c r="BD3" s="20"/>
+      <c r="BE3" s="21"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="26"/>
-      <c r="AF4" s="26"/>
-      <c r="AG4" s="26"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="26"/>
-      <c r="AJ4" s="26"/>
-      <c r="AK4" s="26"/>
-      <c r="AL4" s="26"/>
-      <c r="AM4" s="26"/>
-      <c r="AN4" s="26"/>
-      <c r="AO4" s="26"/>
-      <c r="AP4" s="26"/>
-      <c r="AQ4" s="26"/>
-      <c r="AR4" s="26"/>
-      <c r="AS4" s="26"/>
-      <c r="AT4" s="26"/>
-      <c r="AU4" s="26"/>
-      <c r="AV4" s="26"/>
-      <c r="AW4" s="26"/>
-      <c r="AX4" s="26"/>
-      <c r="AY4" s="26"/>
-      <c r="AZ4" s="26"/>
-      <c r="BA4" s="26"/>
-      <c r="BB4" s="26"/>
-      <c r="BC4" s="26"/>
-      <c r="BD4" s="26"/>
-      <c r="BE4" s="27"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="23"/>
+      <c r="AM4" s="23"/>
+      <c r="AN4" s="23"/>
+      <c r="AO4" s="23"/>
+      <c r="AP4" s="23"/>
+      <c r="AQ4" s="23"/>
+      <c r="AR4" s="23"/>
+      <c r="AS4" s="23"/>
+      <c r="AT4" s="23"/>
+      <c r="AU4" s="23"/>
+      <c r="AV4" s="23"/>
+      <c r="AW4" s="23"/>
+      <c r="AX4" s="23"/>
+      <c r="AY4" s="23"/>
+      <c r="AZ4" s="23"/>
+      <c r="BA4" s="23"/>
+      <c r="BB4" s="23"/>
+      <c r="BC4" s="23"/>
+      <c r="BD4" s="23"/>
+      <c r="BE4" s="24"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="26"/>
-      <c r="AG5" s="26"/>
-      <c r="AH5" s="26"/>
-      <c r="AI5" s="26"/>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="26"/>
-      <c r="AL5" s="26"/>
-      <c r="AM5" s="26"/>
-      <c r="AN5" s="26"/>
-      <c r="AO5" s="26"/>
-      <c r="AP5" s="26"/>
-      <c r="AQ5" s="26"/>
-      <c r="AR5" s="26"/>
-      <c r="AS5" s="26"/>
-      <c r="AT5" s="26"/>
-      <c r="AU5" s="26"/>
-      <c r="AV5" s="26"/>
-      <c r="AW5" s="26"/>
-      <c r="AX5" s="26"/>
-      <c r="AY5" s="26"/>
-      <c r="AZ5" s="26"/>
-      <c r="BA5" s="26"/>
-      <c r="BB5" s="26"/>
-      <c r="BC5" s="26"/>
-      <c r="BD5" s="26"/>
-      <c r="BE5" s="27"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="23"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="23"/>
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="23"/>
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="23"/>
+      <c r="AL5" s="23"/>
+      <c r="AM5" s="23"/>
+      <c r="AN5" s="23"/>
+      <c r="AO5" s="23"/>
+      <c r="AP5" s="23"/>
+      <c r="AQ5" s="23"/>
+      <c r="AR5" s="23"/>
+      <c r="AS5" s="23"/>
+      <c r="AT5" s="23"/>
+      <c r="AU5" s="23"/>
+      <c r="AV5" s="23"/>
+      <c r="AW5" s="23"/>
+      <c r="AX5" s="23"/>
+      <c r="AY5" s="23"/>
+      <c r="AZ5" s="23"/>
+      <c r="BA5" s="23"/>
+      <c r="BB5" s="23"/>
+      <c r="BC5" s="23"/>
+      <c r="BD5" s="23"/>
+      <c r="BE5" s="24"/>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
-      <c r="AG6" s="26"/>
-      <c r="AH6" s="26"/>
-      <c r="AI6" s="26"/>
-      <c r="AJ6" s="26"/>
-      <c r="AK6" s="26"/>
-      <c r="AL6" s="26"/>
-      <c r="AM6" s="26"/>
-      <c r="AN6" s="26"/>
-      <c r="AO6" s="26"/>
-      <c r="AP6" s="26"/>
-      <c r="AQ6" s="26"/>
-      <c r="AR6" s="26"/>
-      <c r="AS6" s="26"/>
-      <c r="AT6" s="26"/>
-      <c r="AU6" s="26"/>
-      <c r="AV6" s="26"/>
-      <c r="AW6" s="26"/>
-      <c r="AX6" s="26"/>
-      <c r="AY6" s="26"/>
-      <c r="AZ6" s="26"/>
-      <c r="BA6" s="26"/>
-      <c r="BB6" s="26"/>
-      <c r="BC6" s="26"/>
-      <c r="BD6" s="26"/>
-      <c r="BE6" s="27"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
+      <c r="AI6" s="23"/>
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="23"/>
+      <c r="AL6" s="23"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="23"/>
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="23"/>
+      <c r="AQ6" s="23"/>
+      <c r="AR6" s="23"/>
+      <c r="AS6" s="23"/>
+      <c r="AT6" s="23"/>
+      <c r="AU6" s="23"/>
+      <c r="AV6" s="23"/>
+      <c r="AW6" s="23"/>
+      <c r="AX6" s="23"/>
+      <c r="AY6" s="23"/>
+      <c r="AZ6" s="23"/>
+      <c r="BA6" s="23"/>
+      <c r="BB6" s="23"/>
+      <c r="BC6" s="23"/>
+      <c r="BD6" s="23"/>
+      <c r="BE6" s="24"/>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.35">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="22"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="22"/>
-      <c r="AD7" s="22"/>
-      <c r="AE7" s="22"/>
-      <c r="AF7" s="22"/>
-      <c r="AG7" s="22"/>
-      <c r="AH7" s="22"/>
-      <c r="AI7" s="22"/>
-      <c r="AJ7" s="22"/>
-      <c r="AK7" s="22"/>
-      <c r="AL7" s="22"/>
-      <c r="AM7" s="22"/>
-      <c r="AN7" s="22"/>
-      <c r="AO7" s="22"/>
-      <c r="AP7" s="22"/>
-      <c r="AQ7" s="22"/>
-      <c r="AR7" s="22"/>
-      <c r="AS7" s="22"/>
-      <c r="AT7" s="22"/>
-      <c r="AU7" s="22"/>
-      <c r="AV7" s="22"/>
-      <c r="AW7" s="22"/>
-      <c r="AX7" s="22"/>
-      <c r="AY7" s="22"/>
-      <c r="AZ7" s="22"/>
-      <c r="BA7" s="22"/>
-      <c r="BB7" s="22"/>
-      <c r="BC7" s="22"/>
-      <c r="BD7" s="22"/>
-      <c r="BE7" s="18"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="35"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="35"/>
+      <c r="AB7" s="35"/>
+      <c r="AC7" s="35"/>
+      <c r="AD7" s="35"/>
+      <c r="AE7" s="35"/>
+      <c r="AF7" s="35"/>
+      <c r="AG7" s="35"/>
+      <c r="AH7" s="35"/>
+      <c r="AI7" s="35"/>
+      <c r="AJ7" s="35"/>
+      <c r="AK7" s="35"/>
+      <c r="AL7" s="35"/>
+      <c r="AM7" s="35"/>
+      <c r="AN7" s="35"/>
+      <c r="AO7" s="35"/>
+      <c r="AP7" s="35"/>
+      <c r="AQ7" s="35"/>
+      <c r="AR7" s="35"/>
+      <c r="AS7" s="35"/>
+      <c r="AT7" s="35"/>
+      <c r="AU7" s="35"/>
+      <c r="AV7" s="35"/>
+      <c r="AW7" s="35"/>
+      <c r="AX7" s="35"/>
+      <c r="AY7" s="35"/>
+      <c r="AZ7" s="35"/>
+      <c r="BA7" s="35"/>
+      <c r="BB7" s="35"/>
+      <c r="BC7" s="35"/>
+      <c r="BD7" s="35"/>
+      <c r="BE7" s="36"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.35">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="19" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19" t="s">
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
-      <c r="Y8" s="22"/>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="19" t="s">
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="35"/>
+      <c r="AA8" s="35"/>
+      <c r="AB8" s="35"/>
+      <c r="AC8" s="35"/>
+      <c r="AD8" s="36"/>
+      <c r="AE8" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="AF8" s="19" t="s">
+      <c r="AF8" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="AG8" s="19" t="s">
+      <c r="AG8" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="AH8" s="17" t="s">
+      <c r="AH8" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="AI8" s="22"/>
-      <c r="AJ8" s="22"/>
-      <c r="AK8" s="22"/>
-      <c r="AL8" s="22"/>
-      <c r="AM8" s="22"/>
-      <c r="AN8" s="22"/>
-      <c r="AO8" s="22"/>
-      <c r="AP8" s="22"/>
-      <c r="AQ8" s="22"/>
-      <c r="AR8" s="18"/>
-      <c r="AS8" s="19" t="s">
+      <c r="AI8" s="35"/>
+      <c r="AJ8" s="35"/>
+      <c r="AK8" s="35"/>
+      <c r="AL8" s="35"/>
+      <c r="AM8" s="35"/>
+      <c r="AN8" s="35"/>
+      <c r="AO8" s="35"/>
+      <c r="AP8" s="35"/>
+      <c r="AQ8" s="35"/>
+      <c r="AR8" s="36"/>
+      <c r="AS8" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="AT8" s="17" t="s">
+      <c r="AT8" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="AU8" s="22"/>
-      <c r="AV8" s="22"/>
-      <c r="AW8" s="22"/>
-      <c r="AX8" s="22"/>
-      <c r="AY8" s="22"/>
-      <c r="AZ8" s="18"/>
-      <c r="BA8" s="19" t="s">
+      <c r="AU8" s="35"/>
+      <c r="AV8" s="35"/>
+      <c r="AW8" s="35"/>
+      <c r="AX8" s="35"/>
+      <c r="AY8" s="35"/>
+      <c r="AZ8" s="36"/>
+      <c r="BA8" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="BB8" s="19" t="s">
+      <c r="BB8" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="BC8" s="19" t="s">
+      <c r="BC8" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="BD8" s="19" t="s">
+      <c r="BD8" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="BE8" s="19" t="s">
+      <c r="BE8" s="31" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.35">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="19" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="19" t="s">
+      <c r="I9" s="32"/>
+      <c r="J9" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="19" t="s">
+      <c r="N9" s="36"/>
+      <c r="O9" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="P9" s="17" t="s">
+      <c r="P9" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="19" t="s">
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="U9" s="17" t="s">
+      <c r="U9" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="V9" s="18"/>
-      <c r="W9" s="19" t="s">
+      <c r="V9" s="36"/>
+      <c r="W9" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="X9" s="17" t="s">
+      <c r="X9" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="19" t="s">
+      <c r="Y9" s="36"/>
+      <c r="Z9" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="AA9" s="19" t="s">
+      <c r="AA9" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="AB9" s="17" t="s">
+      <c r="AB9" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="AC9" s="18"/>
-      <c r="AD9" s="19" t="s">
+      <c r="AC9" s="36"/>
+      <c r="AD9" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="AE9" s="21"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="21"/>
-      <c r="AH9" s="19" t="s">
+      <c r="AE9" s="32"/>
+      <c r="AF9" s="32"/>
+      <c r="AG9" s="32"/>
+      <c r="AH9" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="AI9" s="17" t="s">
+      <c r="AI9" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="AJ9" s="22"/>
-      <c r="AK9" s="18"/>
-      <c r="AL9" s="19" t="s">
+      <c r="AJ9" s="35"/>
+      <c r="AK9" s="36"/>
+      <c r="AL9" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="AM9" s="17" t="s">
+      <c r="AM9" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="AN9" s="22"/>
-      <c r="AO9" s="18"/>
-      <c r="AP9" s="19" t="s">
+      <c r="AN9" s="35"/>
+      <c r="AO9" s="36"/>
+      <c r="AP9" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="AQ9" s="19" t="s">
+      <c r="AQ9" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="AR9" s="19" t="s">
+      <c r="AR9" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="AS9" s="21"/>
-      <c r="AT9" s="19" t="s">
+      <c r="AS9" s="32"/>
+      <c r="AT9" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="AU9" s="17" t="s">
+      <c r="AU9" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="AV9" s="22"/>
-      <c r="AW9" s="18"/>
-      <c r="AX9" s="19" t="s">
+      <c r="AV9" s="35"/>
+      <c r="AW9" s="36"/>
+      <c r="AX9" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="AY9" s="17" t="s">
+      <c r="AY9" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AZ9" s="18"/>
-      <c r="BA9" s="21"/>
-      <c r="BB9" s="21"/>
-      <c r="BC9" s="21"/>
-      <c r="BD9" s="21"/>
-      <c r="BE9" s="21"/>
+      <c r="AZ9" s="36"/>
+      <c r="BA9" s="32"/>
+      <c r="BB9" s="32"/>
+      <c r="BC9" s="32"/>
+      <c r="BD9" s="32"/>
+      <c r="BE9" s="32"/>
     </row>
     <row r="10" spans="1:57" ht="87.75" x14ac:dyDescent="0.35">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
       <c r="M10" s="8" t="s">
         <v>133</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="O10" s="20"/>
+      <c r="O10" s="33"/>
       <c r="P10" s="8" t="s">
         <v>131</v>
       </c>
@@ -1921,33 +1921,33 @@
       <c r="S10" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="T10" s="20"/>
+      <c r="T10" s="33"/>
       <c r="U10" s="8" t="s">
         <v>127</v>
       </c>
       <c r="V10" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="W10" s="20"/>
+      <c r="W10" s="33"/>
       <c r="X10" s="8" t="s">
         <v>125</v>
       </c>
       <c r="Y10" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="33"/>
       <c r="AB10" s="8" t="s">
         <v>123</v>
       </c>
       <c r="AC10" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="AD10" s="20"/>
-      <c r="AE10" s="20"/>
-      <c r="AF10" s="20"/>
-      <c r="AG10" s="20"/>
-      <c r="AH10" s="20"/>
+      <c r="AD10" s="33"/>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="33"/>
+      <c r="AG10" s="33"/>
+      <c r="AH10" s="33"/>
       <c r="AI10" s="8" t="s">
         <v>121</v>
       </c>
@@ -1957,7 +1957,7 @@
       <c r="AK10" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="AL10" s="20"/>
+      <c r="AL10" s="33"/>
       <c r="AM10" s="8" t="s">
         <v>118</v>
       </c>
@@ -1967,11 +1967,11 @@
       <c r="AO10" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="AP10" s="20"/>
-      <c r="AQ10" s="20"/>
-      <c r="AR10" s="20"/>
-      <c r="AS10" s="20"/>
-      <c r="AT10" s="20"/>
+      <c r="AP10" s="33"/>
+      <c r="AQ10" s="33"/>
+      <c r="AR10" s="33"/>
+      <c r="AS10" s="33"/>
+      <c r="AT10" s="33"/>
       <c r="AU10" s="8" t="s">
         <v>115</v>
       </c>
@@ -1981,18 +1981,18 @@
       <c r="AW10" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AX10" s="20"/>
+      <c r="AX10" s="33"/>
       <c r="AY10" s="8" t="s">
         <v>112</v>
       </c>
       <c r="AZ10" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="BA10" s="20"/>
-      <c r="BB10" s="20"/>
-      <c r="BC10" s="20"/>
-      <c r="BD10" s="20"/>
-      <c r="BE10" s="20"/>
+      <c r="BA10" s="33"/>
+      <c r="BB10" s="33"/>
+      <c r="BC10" s="33"/>
+      <c r="BD10" s="33"/>
+      <c r="BE10" s="33"/>
     </row>
     <row r="11" spans="1:57" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A11" s="9" t="s">
@@ -12900,12 +12900,39 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:BE3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:BE4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:BE5"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="BB8:BB10"/>
+    <mergeCell ref="BC8:BC10"/>
+    <mergeCell ref="BD8:BD10"/>
+    <mergeCell ref="BE8:BE10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="AH9:AH10"/>
+    <mergeCell ref="AI9:AK9"/>
+    <mergeCell ref="AL9:AL10"/>
+    <mergeCell ref="AM9:AO9"/>
+    <mergeCell ref="BA8:BA10"/>
+    <mergeCell ref="AY9:AZ9"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AW9"/>
+    <mergeCell ref="AX9:AX10"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:BE6"/>
     <mergeCell ref="A7:B10"/>
@@ -12922,39 +12949,12 @@
     <mergeCell ref="AH8:AR8"/>
     <mergeCell ref="AS8:AS10"/>
     <mergeCell ref="AT8:AZ8"/>
-    <mergeCell ref="AH9:AH10"/>
-    <mergeCell ref="AI9:AK9"/>
-    <mergeCell ref="AL9:AL10"/>
-    <mergeCell ref="AM9:AO9"/>
-    <mergeCell ref="BA8:BA10"/>
-    <mergeCell ref="AY9:AZ9"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AW9"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="BB8:BB10"/>
-    <mergeCell ref="BC8:BC10"/>
-    <mergeCell ref="BD8:BD10"/>
-    <mergeCell ref="BE8:BE10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:BE3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:BE4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:BE5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=TIM_2019_MAIN&amp;ShowOnWeb=true&amp;Lang=en"/>
@@ -12981,7 +12981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK63"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A38" sqref="A38:XFD41"/>
     </sheetView>
   </sheetViews>
@@ -22414,7 +22414,7 @@
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AK2"/>
+      <selection activeCell="B2" sqref="B2:AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22542,148 +22542,148 @@
         <v>BRA: Brazil</v>
       </c>
       <c r="B2">
-        <f>'Filtered OECD Data'!B41</f>
-        <v>13137.5</v>
+        <f>'Filtered OECD Data'!B41*1000</f>
+        <v>13137500</v>
       </c>
       <c r="C2">
-        <f>'Filtered OECD Data'!C41</f>
-        <v>12.5</v>
+        <f>'Filtered OECD Data'!C41*1000</f>
+        <v>12500</v>
       </c>
       <c r="D2">
-        <f>'Filtered OECD Data'!D41</f>
-        <v>211.8</v>
+        <f>'Filtered OECD Data'!D41*1000</f>
+        <v>211800</v>
       </c>
       <c r="E2">
-        <f>'Filtered OECD Data'!E41</f>
-        <v>63.2</v>
+        <f>'Filtered OECD Data'!E41*1000</f>
+        <v>63200</v>
       </c>
       <c r="F2">
-        <f>'Filtered OECD Data'!F41</f>
-        <v>2365.8000000000002</v>
+        <f>'Filtered OECD Data'!F41*1000</f>
+        <v>2365800</v>
       </c>
       <c r="G2">
-        <f>'Filtered OECD Data'!G41</f>
-        <v>2803.2</v>
+        <f>'Filtered OECD Data'!G41*1000</f>
+        <v>2803200</v>
       </c>
       <c r="H2">
-        <f>'Filtered OECD Data'!H41</f>
-        <v>381.7</v>
+        <f>'Filtered OECD Data'!H41*1000</f>
+        <v>381700</v>
       </c>
       <c r="I2">
-        <f>'Filtered OECD Data'!I41</f>
-        <v>400.7</v>
+        <f>'Filtered OECD Data'!I41*1000</f>
+        <v>400700</v>
       </c>
       <c r="J2">
-        <f>'Filtered OECD Data'!J41</f>
-        <v>23.1</v>
+        <f>'Filtered OECD Data'!J41*1000</f>
+        <v>23100</v>
       </c>
       <c r="K2">
-        <f>'Filtered OECD Data'!K41</f>
-        <v>546.1</v>
+        <f>'Filtered OECD Data'!K41*1000</f>
+        <v>546100</v>
       </c>
       <c r="L2">
-        <f>'Filtered OECD Data'!L41</f>
-        <v>446</v>
+        <f>'Filtered OECD Data'!L41*1000</f>
+        <v>446000</v>
       </c>
       <c r="M2">
-        <f>'Filtered OECD Data'!M41</f>
-        <v>654</v>
+        <f>'Filtered OECD Data'!M41*1000</f>
+        <v>654000</v>
       </c>
       <c r="N2">
-        <f>'Filtered OECD Data'!N41</f>
-        <v>224.7</v>
+        <f>'Filtered OECD Data'!N41*1000</f>
+        <v>224700</v>
       </c>
       <c r="O2">
-        <f>'Filtered OECD Data'!O41</f>
-        <v>724.8</v>
+        <f>'Filtered OECD Data'!O41*1000</f>
+        <v>724800</v>
       </c>
       <c r="P2">
-        <f>'Filtered OECD Data'!P41</f>
-        <v>144</v>
+        <f>'Filtered OECD Data'!P41*1000</f>
+        <v>144000</v>
       </c>
       <c r="Q2">
-        <f>'Filtered OECD Data'!Q41</f>
-        <v>222.9</v>
+        <f>'Filtered OECD Data'!Q41*1000</f>
+        <v>222900</v>
       </c>
       <c r="R2">
-        <f>'Filtered OECD Data'!R41</f>
-        <v>410</v>
+        <f>'Filtered OECD Data'!R41*1000</f>
+        <v>410000</v>
       </c>
       <c r="S2">
-        <f>'Filtered OECD Data'!S41</f>
-        <v>457.4</v>
+        <f>'Filtered OECD Data'!S41*1000</f>
+        <v>457400</v>
       </c>
       <c r="T2">
-        <f>'Filtered OECD Data'!T41</f>
-        <v>114.1</v>
+        <f>'Filtered OECD Data'!T41*1000</f>
+        <v>114100</v>
       </c>
       <c r="U2">
-        <f>'Filtered OECD Data'!U41</f>
-        <v>1294.9000000000001</v>
+        <f>'Filtered OECD Data'!U41*1000</f>
+        <v>1294900</v>
       </c>
       <c r="V2">
-        <f>'Filtered OECD Data'!V41</f>
-        <v>677.4</v>
+        <f>'Filtered OECD Data'!V41*1000</f>
+        <v>677400</v>
       </c>
       <c r="W2">
-        <f>'Filtered OECD Data'!W41</f>
-        <v>8639.9</v>
+        <f>'Filtered OECD Data'!W41*1000</f>
+        <v>8639900</v>
       </c>
       <c r="X2">
-        <f>'Filtered OECD Data'!X41</f>
-        <v>18873.400000000001</v>
+        <f>'Filtered OECD Data'!X41*1000</f>
+        <v>18873400</v>
       </c>
       <c r="Y2">
-        <f>'Filtered OECD Data'!Y41</f>
-        <v>4711.1000000000004</v>
+        <f>'Filtered OECD Data'!Y41*1000</f>
+        <v>4711100</v>
       </c>
       <c r="Z2">
-        <f>'Filtered OECD Data'!Z41</f>
-        <v>5386</v>
+        <f>'Filtered OECD Data'!Z41*1000</f>
+        <v>5386000</v>
       </c>
       <c r="AA2">
-        <f>'Filtered OECD Data'!AA41</f>
-        <v>341.2</v>
+        <f>'Filtered OECD Data'!AA41*1000</f>
+        <v>341200</v>
       </c>
       <c r="AB2">
-        <f>'Filtered OECD Data'!AB41</f>
-        <v>233.3</v>
+        <f>'Filtered OECD Data'!AB41*1000</f>
+        <v>233300</v>
       </c>
       <c r="AC2">
-        <f>'Filtered OECD Data'!AC41</f>
-        <v>775.2</v>
+        <f>'Filtered OECD Data'!AC41*1000</f>
+        <v>775200</v>
       </c>
       <c r="AD2">
-        <f>'Filtered OECD Data'!AD41</f>
-        <v>1199.9000000000001</v>
+        <f>'Filtered OECD Data'!AD41*1000</f>
+        <v>1199900</v>
       </c>
       <c r="AE2">
-        <f>'Filtered OECD Data'!AE41</f>
-        <v>417.1</v>
+        <f>'Filtered OECD Data'!AE41*1000</f>
+        <v>417100</v>
       </c>
       <c r="AF2">
-        <f>'Filtered OECD Data'!AF41</f>
-        <v>8124.3</v>
+        <f>'Filtered OECD Data'!AF41*1000</f>
+        <v>8124300</v>
       </c>
       <c r="AG2">
-        <f>'Filtered OECD Data'!AG41</f>
-        <v>5093.3</v>
+        <f>'Filtered OECD Data'!AG41*1000</f>
+        <v>5093300</v>
       </c>
       <c r="AH2">
-        <f>'Filtered OECD Data'!AH41</f>
-        <v>6655.2</v>
+        <f>'Filtered OECD Data'!AH41*1000</f>
+        <v>6655200</v>
       </c>
       <c r="AI2">
-        <f>'Filtered OECD Data'!AI41</f>
-        <v>4811.8</v>
+        <f>'Filtered OECD Data'!AI41*1000</f>
+        <v>4811800</v>
       </c>
       <c r="AJ2">
-        <f>'Filtered OECD Data'!AJ41</f>
-        <v>4986.2</v>
+        <f>'Filtered OECD Data'!AJ41*1000</f>
+        <v>4986200</v>
       </c>
       <c r="AK2">
-        <f>'Filtered OECD Data'!AK41</f>
-        <v>6381.2</v>
+        <f>'Filtered OECD Data'!AK41*1000</f>
+        <v>6381200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>